<commit_message>
add new literature day 1
</commit_message>
<xml_diff>
--- a/1_pages/files/Workshop-Participants-Contact-Information.xlsx
+++ b/1_pages/files/Workshop-Participants-Contact-Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassi\Documents\GitHub\AB-RCSC\test_alif2499\1_pages\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassi\Documents\GitHub\AB-RCSC\GOA_Ungulate-monitoring-methods-workshop\1_pages\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB72909-E3DA-4575-8303-55E5AE36FCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE30114-36A6-407E-8DBF-285CF32AC5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="9" r:id="rId1"/>
@@ -698,9 +698,6 @@
     <t>tgraves@usgs.gov</t>
   </si>
   <si>
-    <t>Daniel  Melody</t>
-  </si>
-  <si>
     <t>Wildlife Biologist / Operations Manager</t>
   </si>
   <si>
@@ -728,9 +725,6 @@
     <t>Senior Environmental Scientist Supervisor</t>
   </si>
   <si>
-    <t>Lalenia  Neufeld</t>
-  </si>
-  <si>
     <t>lalenia.neufeld@pc.gc.ca</t>
   </si>
   <si>
@@ -2052,6 +2046,12 @@
   </si>
   <si>
     <t>BC Ministry of WLRS - Terrestrial Species Recovery Branch</t>
+  </si>
+  <si>
+    <t>Lalenia Neufeld</t>
+  </si>
+  <si>
+    <t>Daniel Melody</t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2322,6 +2322,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -3030,9 +3033,9 @@
   </sheetPr>
   <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3056,7 +3059,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>2</v>
@@ -3068,7 +3071,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H1" s="28" t="s">
         <v>5</v>
@@ -3076,25 +3079,25 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>464</v>
-      </c>
       <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>168</v>
@@ -3111,10 +3114,10 @@
         <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>7</v>
@@ -3123,7 +3126,7 @@
         <v>66</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3131,10 +3134,10 @@
         <v>110</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>111</v>
@@ -3146,7 +3149,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>18</v>
@@ -3154,19 +3157,19 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>329</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>7</v>
@@ -3175,30 +3178,30 @@
         <v>66</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>18</v>
@@ -3206,25 +3209,25 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>483</v>
-      </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>18</v>
@@ -3232,19 +3235,19 @@
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>7</v>
@@ -3253,7 +3256,7 @@
         <v>66</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3264,7 +3267,7 @@
         <v>60</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>61</v>
@@ -3276,7 +3279,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>10</v>
@@ -3284,25 +3287,25 @@
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>426</v>
-      </c>
       <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>168</v>
@@ -3310,25 +3313,25 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>560</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>522</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>254</v>
-      </c>
       <c r="F11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>18</v>
@@ -3336,7 +3339,7 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>49</v>
@@ -3345,24 +3348,24 @@
         <v>155</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>20</v>
@@ -3371,10 +3374,10 @@
         <v>65</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>7</v>
@@ -3383,30 +3386,30 @@
         <v>66</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>18</v>
@@ -3432,27 +3435,27 @@
         <v>9</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>7</v>
@@ -3461,30 +3464,30 @@
         <v>66</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>639</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>416</v>
-      </c>
       <c r="F17" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>18</v>
@@ -3510,53 +3513,53 @@
         <v>9</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>651</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>381</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>7</v>
@@ -3565,24 +3568,24 @@
         <v>66</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>229</v>
-      </c>
       <c r="C21" s="7" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>7</v>
@@ -3591,30 +3594,30 @@
         <v>8</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>95</v>
@@ -3622,77 +3625,77 @@
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>564</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>640</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>293</v>
-      </c>
       <c r="F23" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>565</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>614</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>489</v>
-      </c>
       <c r="F24" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>566</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>567</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>266</v>
-      </c>
       <c r="F25" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>18</v>
@@ -3700,25 +3703,25 @@
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>95</v>
@@ -3729,10 +3732,10 @@
         <v>96</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>97</v>
@@ -3744,7 +3747,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>18</v>
@@ -3755,10 +3758,10 @@
         <v>96</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>97</v>
@@ -3770,7 +3773,7 @@
         <v>9</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>18</v>
@@ -3778,25 +3781,25 @@
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>133</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>18</v>
@@ -3804,7 +3807,7 @@
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>49</v>
@@ -3813,7 +3816,7 @@
         <v>155</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>156</v>
@@ -3822,7 +3825,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>95</v>
@@ -3848,7 +3851,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>18</v>
@@ -3874,33 +3877,33 @@
         <v>9</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>625</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>410</v>
-      </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>18</v>
@@ -3914,7 +3917,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>21</v>
@@ -3926,59 +3929,59 @@
         <v>9</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>18</v>
@@ -3986,25 +3989,25 @@
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>18</v>
@@ -4012,25 +4015,25 @@
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>165</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>168</v>
@@ -4038,45 +4041,45 @@
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="C40" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>573</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>222</v>
-      </c>
       <c r="E40" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>7</v>
@@ -4085,7 +4088,7 @@
         <v>14</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4093,7 +4096,7 @@
         <v>23</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>155</v>
@@ -4108,33 +4111,33 @@
         <v>9</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="E42" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>420</v>
-      </c>
       <c r="F42" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H42" s="17" t="s">
         <v>95</v>
@@ -4142,7 +4145,7 @@
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>20</v>
@@ -4151,16 +4154,16 @@
         <v>155</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>95</v>
@@ -4189,24 +4192,24 @@
         <v>14</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>7</v>
@@ -4215,108 +4218,108 @@
         <v>14</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="D46" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>444</v>
-      </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="E47" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="E48" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>280</v>
-      </c>
       <c r="F48" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H49" s="17" t="s">
         <v>18</v>
@@ -4324,7 +4327,7 @@
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>20</v>
@@ -4333,16 +4336,16 @@
         <v>67</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H50" s="18" t="s">
         <v>18</v>
@@ -4350,25 +4353,25 @@
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H51" s="17" t="s">
         <v>18</v>
@@ -4376,28 +4379,28 @@
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="D52" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="E52" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>456</v>
-      </c>
       <c r="F52" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4408,7 +4411,7 @@
         <v>130</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>27</v>
@@ -4420,15 +4423,15 @@
         <v>9</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>20</v>
@@ -4437,16 +4440,16 @@
         <v>155</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H54" s="17" t="s">
         <v>95</v>
@@ -4460,22 +4463,22 @@
         <v>20</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4486,7 +4489,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>46</v>
@@ -4498,33 +4501,33 @@
         <v>9</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H57" s="17" t="s">
         <v>168</v>
@@ -4538,7 +4541,7 @@
         <v>30</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>31</v>
@@ -4550,33 +4553,33 @@
         <v>9</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="E59" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>645</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>468</v>
-      </c>
       <c r="F59" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H59" s="17" t="s">
         <v>168</v>
@@ -4590,7 +4593,7 @@
         <v>41</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>42</v>
@@ -4602,10 +4605,10 @@
         <v>9</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4628,7 +4631,7 @@
         <v>9</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H61" s="17" t="s">
         <v>95</v>
@@ -4636,28 +4639,28 @@
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="E62" s="8" t="s">
         <v>478</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>628</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>480</v>
-      </c>
       <c r="F62" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4671,7 +4674,7 @@
         <v>179</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>180</v>
@@ -4680,7 +4683,7 @@
         <v>9</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H63" s="17" t="s">
         <v>18</v>
@@ -4688,28 +4691,28 @@
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="E64" s="8" t="s">
         <v>494</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>495</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>496</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H64" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4720,19 +4723,19 @@
         <v>57</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H65" s="17" t="s">
         <v>10</v>
@@ -4743,22 +4746,22 @@
         <v>212</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>213</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H66" s="17" t="s">
         <v>18</v>
@@ -4766,25 +4769,25 @@
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>577</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>631</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>486</v>
-      </c>
       <c r="F67" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H67" s="17" t="s">
         <v>95</v>
@@ -4792,16 +4795,16 @@
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>55</v>
@@ -4810,7 +4813,7 @@
         <v>9</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H68" s="17" t="s">
         <v>10</v>
@@ -4836,7 +4839,7 @@
         <v>9</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H69" s="17" t="s">
         <v>18</v>
@@ -4844,28 +4847,28 @@
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="E70" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>372</v>
-      </c>
       <c r="F70" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4873,25 +4876,25 @@
         <v>77</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4899,7 +4902,7 @@
         <v>201</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>202</v>
@@ -4908,13 +4911,13 @@
         <v>203</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H72" s="17" t="s">
         <v>18</v>
@@ -4925,10 +4928,10 @@
         <v>11</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>12</v>
@@ -4943,12 +4946,12 @@
         <v>14</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>125</v>
@@ -4966,10 +4969,10 @@
         <v>9</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4986,7 +4989,7 @@
         <v>200</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>7</v>
@@ -4995,33 +4998,33 @@
         <v>66</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="E76" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B76" s="7" t="s">
-        <v>583</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>260</v>
-      </c>
       <c r="F76" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5032,7 +5035,7 @@
         <v>37</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>38</v>
@@ -5044,27 +5047,27 @@
         <v>9</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>7</v>
@@ -5073,56 +5076,56 @@
         <v>66</v>
       </c>
       <c r="H78" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B79" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="D79" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="E79" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="H79" s="17" t="s">
         <v>226</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>519</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G79" s="8" t="s">
-        <v>519</v>
-      </c>
-      <c r="H79" s="17" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="E80" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>433</v>
-      </c>
       <c r="F80" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H80" s="17" t="s">
         <v>168</v>
@@ -5142,42 +5145,42 @@
         <v>154</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>631</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>257</v>
-      </c>
       <c r="F82" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H82" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5185,7 +5188,7 @@
         <v>204</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>205</v>
@@ -5194,7 +5197,7 @@
         <v>206</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>7</v>
@@ -5203,30 +5206,30 @@
         <v>207</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="D84" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="E84" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>613</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>346</v>
-      </c>
       <c r="F84" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H84" s="17" t="s">
         <v>18</v>
@@ -5234,25 +5237,25 @@
     </row>
     <row r="85" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C85" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="D85" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="E85" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="D85" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>308</v>
-      </c>
       <c r="F85" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H85" s="18" t="s">
         <v>18</v>
@@ -5266,45 +5269,45 @@
         <v>20</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H87" s="17" t="s">
         <v>18</v>
@@ -5312,25 +5315,25 @@
     </row>
     <row r="88" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="E88" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>615</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>650</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>392</v>
-      </c>
       <c r="F88" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H88" s="17" t="s">
         <v>18</v>
@@ -5347,16 +5350,16 @@
         <v>209</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H89" s="17" t="s">
         <v>210</v>
@@ -5376,13 +5379,13 @@
         <v>54</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H90" s="17" t="s">
         <v>18</v>
@@ -5390,77 +5393,77 @@
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="D91" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="E91" s="8" t="s">
         <v>435</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>651</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>437</v>
       </c>
       <c r="F91" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>230</v>
+        <v>670</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>652</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>231</v>
+        <v>650</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>229</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H92" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F93" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H93" s="17" t="s">
         <v>18</v>
@@ -5468,28 +5471,28 @@
     </row>
     <row r="94" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="D94" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="E94" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C94" s="7" t="s">
-        <v>586</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>272</v>
-      </c>
       <c r="F94" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H94" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5512,7 +5515,7 @@
         <v>9</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H95" s="17" t="s">
         <v>168</v>
@@ -5538,7 +5541,7 @@
         <v>9</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H96" s="17" t="s">
         <v>168</v>
@@ -5546,25 +5549,25 @@
     </row>
     <row r="97" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="E97" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="C97" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>472</v>
-      </c>
       <c r="F97" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H97" s="17" t="s">
         <v>18</v>
@@ -5572,25 +5575,25 @@
     </row>
     <row r="98" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H98" s="17" t="s">
         <v>18</v>
@@ -5598,19 +5601,19 @@
     </row>
     <row r="99" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>7</v>
@@ -5619,7 +5622,7 @@
         <v>66</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="100" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5642,7 +5645,7 @@
         <v>9</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H100" s="17" t="s">
         <v>136</v>
@@ -5650,25 +5653,25 @@
     </row>
     <row r="101" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F101" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H101" s="17" t="s">
         <v>18</v>
@@ -5676,25 +5679,25 @@
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F102" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H102" s="17" t="s">
         <v>95</v>
@@ -5708,7 +5711,7 @@
         <v>160</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>161</v>
@@ -5720,7 +5723,7 @@
         <v>9</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>18</v>
@@ -5728,25 +5731,25 @@
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B104" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D104" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C104" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="E104" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F104" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H104" s="17" t="s">
         <v>95</v>
@@ -5754,19 +5757,19 @@
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="D105" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="E105" s="8" t="s">
         <v>405</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>670</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>407</v>
       </c>
       <c r="F105" s="8" t="s">
         <v>7</v>
@@ -5775,7 +5778,7 @@
         <v>66</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5783,7 +5786,7 @@
         <v>68</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>69</v>
@@ -5798,59 +5801,59 @@
         <v>9</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H106" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F107" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H107" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F108" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H108" s="17" t="s">
         <v>168</v>
@@ -5858,45 +5861,45 @@
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F110" s="8" t="s">
         <v>7</v>
@@ -5905,30 +5908,30 @@
         <v>66</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F111" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G111" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>18</v>
@@ -5939,7 +5942,7 @@
         <v>117</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>118</v>
@@ -5948,39 +5951,39 @@
         <v>119</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F112" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G112" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="E113" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="B113" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>671</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>541</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>384</v>
-      </c>
       <c r="F113" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G113" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>18</v>
@@ -5988,28 +5991,28 @@
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F114" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6032,7 +6035,7 @@
         <v>9</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>18</v>
@@ -6046,7 +6049,7 @@
         <v>20</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>93</v>
@@ -6058,7 +6061,7 @@
         <v>9</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>95</v>
@@ -6066,25 +6069,25 @@
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F117" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G117" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>18</v>
@@ -6098,10 +6101,10 @@
         <v>49</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>50</v>
@@ -6110,27 +6113,27 @@
         <v>9</v>
       </c>
       <c r="G118" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="D119" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="E119" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="F119" s="8" t="s">
         <v>7</v>
@@ -6139,30 +6142,30 @@
         <v>66</v>
       </c>
       <c r="H119" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="D120" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="E120" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="C120" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="E120" s="8" t="s">
-        <v>476</v>
-      </c>
       <c r="F120" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G120" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>18</v>
@@ -6176,10 +6179,10 @@
         <v>130</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>131</v>
@@ -6188,7 +6191,7 @@
         <v>9</v>
       </c>
       <c r="G121" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>95</v>
@@ -6196,7 +6199,7 @@
     </row>
     <row r="122" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>34</v>
@@ -6205,10 +6208,10 @@
         <v>65</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F122" s="8" t="s">
         <v>7</v>
@@ -6217,7 +6220,7 @@
         <v>66</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6240,10 +6243,10 @@
         <v>9</v>
       </c>
       <c r="G123" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6251,16 +6254,16 @@
         <v>157</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>158</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F124" s="8" t="s">
         <v>7</v>
@@ -6269,30 +6272,30 @@
         <v>66</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="D125" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="B125" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>634</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>349</v>
-      </c>
       <c r="E125" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F125" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G125" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H125" s="17" t="s">
         <v>18</v>
@@ -6300,7 +6303,7 @@
     </row>
     <row r="126" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>99</v>
@@ -6318,85 +6321,85 @@
         <v>9</v>
       </c>
       <c r="G126" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="127" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F127" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G127" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B128" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="E128" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="C128" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>429</v>
-      </c>
       <c r="F128" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G128" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B129" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F129" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G129" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H129" s="17" t="s">
         <v>18</v>
@@ -6404,25 +6407,25 @@
     </row>
     <row r="130" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B130" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C130" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="D130" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="E130" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="D130" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="E130" s="12" t="s">
-        <v>333</v>
-      </c>
       <c r="F130" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G130" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H130" s="18" t="s">
         <v>18</v>
@@ -6430,10 +6433,10 @@
     </row>
     <row r="131" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>214</v>
@@ -6442,7 +6445,7 @@
         <v>215</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F131" s="8" t="s">
         <v>7</v>
@@ -6451,7 +6454,7 @@
         <v>216</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6462,19 +6465,19 @@
         <v>20</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>182</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F132" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H132" s="17" t="s">
         <v>18</v>
@@ -6482,19 +6485,19 @@
     </row>
     <row r="133" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F133" s="8" t="s">
         <v>7</v>
@@ -6503,30 +6506,30 @@
         <v>66</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B134" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F134" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G134" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H134" s="17" t="s">
         <v>210</v>
@@ -6540,7 +6543,7 @@
         <v>20</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>147</v>
@@ -6552,10 +6555,10 @@
         <v>9</v>
       </c>
       <c r="G135" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H135" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6566,10 +6569,10 @@
         <v>16</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>17</v>
@@ -6578,7 +6581,7 @@
         <v>9</v>
       </c>
       <c r="G136" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H136" s="17" t="s">
         <v>18</v>
@@ -6586,7 +6589,7 @@
     </row>
     <row r="137" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>20</v>
@@ -6595,16 +6598,16 @@
         <v>165</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E137" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F137" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H137" s="17" t="s">
         <v>18</v>
@@ -6612,28 +6615,28 @@
     </row>
     <row r="138" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>155</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F138" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H138" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6650,39 +6653,39 @@
         <v>105</v>
       </c>
       <c r="E139" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G139" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H139" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="E140" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="B140" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="D140" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="E140" s="8" t="s">
-        <v>403</v>
-      </c>
       <c r="F140" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G140" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H140" s="17" t="s">
         <v>18</v>
@@ -6690,19 +6693,19 @@
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F141" s="8" t="s">
         <v>7</v>
@@ -6711,30 +6714,30 @@
         <v>66</v>
       </c>
       <c r="H141" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C142" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="D142" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="E142" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="D142" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="E142" s="8" t="s">
-        <v>360</v>
-      </c>
       <c r="F142" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G142" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H142" s="17" t="s">
         <v>18</v>
@@ -6748,10 +6751,10 @@
         <v>34</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>35</v>
@@ -6760,7 +6763,7 @@
         <v>9</v>
       </c>
       <c r="G143" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H143" s="17" t="s">
         <v>10</v>
@@ -6768,25 +6771,25 @@
     </row>
     <row r="144" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B144" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C144" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="D144" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="E144" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="D144" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="E144" s="12" t="s">
-        <v>355</v>
-      </c>
       <c r="F144" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G144" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H144" s="18" t="s">
         <v>18</v>
@@ -6800,7 +6803,7 @@
         <v>20</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D145" s="6" t="s">
         <v>80</v>
@@ -6812,10 +6815,10 @@
         <v>9</v>
       </c>
       <c r="G145" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6826,19 +6829,19 @@
         <v>20</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D146" s="6" t="s">
         <v>173</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F146" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G146" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H146" s="17" t="s">
         <v>10</v>
@@ -6846,25 +6849,25 @@
     </row>
     <row r="147" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F147" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G147" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H147" s="17" t="s">
         <v>95</v>
@@ -6890,33 +6893,33 @@
         <v>9</v>
       </c>
       <c r="G148" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F149" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G149" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H149" s="17" t="s">
         <v>18</v>
@@ -6930,19 +6933,19 @@
         <v>175</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>176</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F150" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G150" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H150" s="17" t="s">
         <v>18</v>
@@ -6956,13 +6959,13 @@
         <v>218</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>219</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F151" s="8" t="s">
         <v>7</v>
@@ -6971,7 +6974,7 @@
         <v>66</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6997,7 +7000,7 @@
         <v>14</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -7005,7 +7008,7 @@
         <v>132</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>133</v>
@@ -7020,27 +7023,27 @@
         <v>9</v>
       </c>
       <c r="G153" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H153" s="17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D154" s="13" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E154" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F154" s="8" t="s">
         <v>7</v>
@@ -7049,30 +7052,30 @@
         <v>8</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="155" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C155" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="B155" s="11" t="s">
+      <c r="D155" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="E155" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="D155" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="E155" s="12" t="s">
-        <v>342</v>
-      </c>
       <c r="F155" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G155" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H155" s="18" t="s">
         <v>18</v>
@@ -7083,22 +7086,22 @@
         <v>211</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>209</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E156" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F156" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G156" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H156" s="17" t="s">
         <v>210</v>
@@ -7106,25 +7109,25 @@
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="E157" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="B157" s="7" t="s">
-        <v>458</v>
-      </c>
-      <c r="C157" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>552</v>
-      </c>
-      <c r="E157" s="8" t="s">
-        <v>459</v>
-      </c>
       <c r="F157" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G157" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H157" s="17" t="s">
         <v>10</v>
@@ -7132,77 +7135,77 @@
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C158" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E158" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="D158" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>263</v>
-      </c>
       <c r="F158" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G158" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>155</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F159" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G159" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H159" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="160" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="D160" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="B160" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>492</v>
-      </c>
       <c r="E160" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F160" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G160" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H160" s="17" t="s">
         <v>18</v>
@@ -7210,25 +7213,25 @@
     </row>
     <row r="161" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="16" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E161" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F161" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G161" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H161" s="18" t="s">
         <v>18</v>
@@ -7242,7 +7245,7 @@
         <v>20</v>
       </c>
       <c r="C162" s="20" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>88</v>
@@ -7254,7 +7257,7 @@
         <v>9</v>
       </c>
       <c r="G162" s="22" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H162" s="23" t="s">
         <v>18</v>
@@ -7269,14 +7272,16 @@
     <hyperlink ref="D50" r:id="rId2" xr:uid="{19E1CC45-80AB-439D-AF63-C3EB19FD826F}"/>
     <hyperlink ref="D101" r:id="rId3" display="Luke.VanderVennen@gov.bc.ca" xr:uid="{6EE77E3B-1361-409F-947E-B7652023C88A}"/>
     <hyperlink ref="D154" r:id="rId4" display="Thomas.Connor@wildlife.ca.gov" xr:uid="{9EAE1316-863D-4659-9E53-BFF9CA6F2E9C}"/>
+    <hyperlink ref="D92" r:id="rId5" xr:uid="{9D24B52A-64E1-424F-8B09-014379F68139}"/>
+    <hyperlink ref="D40" r:id="rId6" xr:uid="{74BF6D27-4A36-4422-808F-658D131F21A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;11&amp;K000000 Classification: Protected A</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>